<commit_message>
agregando ejercicio de pensiones y longevidad
</commit_message>
<xml_diff>
--- a/src/TM_hombres.xlsx
+++ b/src/TM_hombres.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ximena Quiroga\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace_github\PJ_TEMPLATE\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{501EBC58-D55F-4028-AB9F-F048AEF1CC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0332FAB-DB4C-4641-8F9B-400A88E0A224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{13277F8B-6E91-4C57-83B1-9DA2076F8607}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{13277F8B-6E91-4C57-83B1-9DA2076F8607}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -95,12 +95,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -438,15 +437,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E167C9F9-D58C-457B-868D-655D64A2EFB3}">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,1635 +464,1635 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>1000000</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>485</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>4.8500000000000003E-4</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>64.8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>16</v>
       </c>
       <c r="B3" s="1">
         <v>999515</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>496</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>4.9600000000000002E-4</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
         <v>63.9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>17</v>
       </c>
       <c r="B4" s="1">
         <v>999019</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>509</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <v>5.0900000000000001E-4</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <v>62.9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>18</v>
       </c>
       <c r="B5" s="1">
         <v>998510</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>522</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>5.2300000000000003E-4</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <v>61.9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>19</v>
       </c>
       <c r="B6" s="1">
         <v>997988</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>537</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <v>5.3799999999999996E-4</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <v>60.9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>20</v>
       </c>
       <c r="B7" s="1">
-        <v>997.45100000000002</v>
-      </c>
-      <c r="C7" s="2">
+        <v>997451</v>
+      </c>
+      <c r="C7">
         <v>553</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <v>5.5400000000000002E-4</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>21</v>
       </c>
       <c r="B8" s="1">
         <v>996898</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>571</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8">
         <v>5.7300000000000005E-4</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>22</v>
       </c>
       <c r="B9" s="1">
         <v>996327</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
         <v>591</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9">
         <v>5.9299999999999999E-4</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>23</v>
       </c>
       <c r="B10" s="1">
         <v>995736</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10">
         <v>612</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10">
         <v>6.1499999999999999E-4</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10">
         <v>57.1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>24</v>
       </c>
       <c r="B11" s="1">
         <v>995124</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
         <v>636</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11">
         <v>6.3900000000000003E-4</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11">
         <v>56.1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>25</v>
       </c>
       <c r="B12" s="1">
         <v>994488</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12">
         <v>662</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12">
         <v>6.6600000000000003E-4</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12">
         <v>55.1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>26</v>
       </c>
       <c r="B13" s="1">
         <v>993826</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13">
         <v>690</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13">
         <v>6.9399999999999996E-4</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13">
         <v>54.2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>27</v>
       </c>
       <c r="B14" s="1">
         <v>993136</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14">
         <v>721</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14">
         <v>7.2599999999999997E-4</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14">
         <v>53.2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>28</v>
       </c>
       <c r="B15" s="1">
         <v>992415</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15">
         <v>755</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15">
         <v>7.6099999999999996E-4</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15">
         <v>52.3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>29</v>
       </c>
       <c r="B16" s="1">
         <v>991660</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16">
         <v>792</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16">
         <v>7.9900000000000001E-4</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16">
         <v>51.3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>30</v>
       </c>
       <c r="B17" s="1">
         <v>990868</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17">
         <v>832</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17">
         <v>8.4000000000000003E-4</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17">
         <v>50.3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>990036</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18">
         <v>877</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18">
         <v>8.8599999999999996E-4</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18">
         <v>49.4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>32</v>
       </c>
       <c r="B19" s="1">
         <v>989159</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19">
         <v>926</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19">
         <v>9.3599999999999998E-4</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19">
         <v>48.4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>33</v>
       </c>
       <c r="B20" s="1">
         <v>988233</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20">
         <v>979</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20">
         <v>9.9099999999999991E-4</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20">
         <v>47.5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>34</v>
       </c>
       <c r="B21" s="1">
         <v>987254</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21">
         <v>1038</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21">
         <v>1.0510000000000001E-3</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21">
         <v>46.5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>35</v>
       </c>
       <c r="B22" s="1">
         <v>986216</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22">
         <v>1102</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22">
         <v>1.1169999999999999E-3</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22">
         <v>45.6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>36</v>
       </c>
       <c r="B23" s="1">
         <v>985114</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23">
         <v>1172</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23">
         <v>1.1900000000000001E-3</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23">
         <v>44.6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>37</v>
       </c>
       <c r="B24" s="1">
         <v>983942</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24">
         <v>1249</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24">
         <v>1.2689999999999999E-3</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24">
         <v>43.7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>38</v>
       </c>
       <c r="B25" s="1">
         <v>982693</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25">
         <v>1333</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25">
         <v>1.356E-3</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25">
         <v>42.7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>39</v>
       </c>
       <c r="B26" s="1">
         <v>981360</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26">
         <v>1424</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26">
         <v>1.451E-3</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26">
         <v>41.8</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>40</v>
       </c>
       <c r="B27" s="1">
         <v>979936</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27">
         <v>1525</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27">
         <v>1.5560000000000001E-3</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27">
         <v>40.799999999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>41</v>
       </c>
       <c r="B28" s="1">
         <v>978411</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28">
         <v>1635</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28">
         <v>1.671E-3</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28">
         <v>39.9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>42</v>
       </c>
       <c r="B29" s="1">
         <v>976776</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29">
         <v>1755</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29">
         <v>1.797E-3</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>43</v>
       </c>
       <c r="B30" s="1">
         <v>975021</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30">
         <v>1886</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30">
         <v>1.934E-3</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>44</v>
       </c>
       <c r="B31" s="1">
         <v>973135</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31">
         <v>2030</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31">
         <v>2.0860000000000002E-3</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31">
         <v>37.1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>45</v>
       </c>
       <c r="B32" s="1">
         <v>971105</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32">
         <v>2186</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32">
         <v>2.251E-3</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32">
         <v>36.200000000000003</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>46</v>
       </c>
       <c r="B33" s="1">
         <v>968919</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33">
         <v>2358</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33">
         <v>2.434E-3</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33">
         <v>35.299999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>47</v>
       </c>
       <c r="B34" s="1">
         <v>966561</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34">
         <v>2544</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34">
         <v>2.6319999999999998E-3</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34">
         <v>34.4</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>48</v>
       </c>
       <c r="B35" s="1">
         <v>964017</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35">
         <v>2748</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35">
         <v>2.8509999999999998E-3</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35">
         <v>33.4</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>49</v>
       </c>
       <c r="B36" s="1">
         <v>961269</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36">
         <v>2971</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36">
         <v>3.091E-3</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36">
         <v>32.5</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>50</v>
       </c>
       <c r="B37" s="1">
         <v>958298</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37">
         <v>3213</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37">
         <v>3.3530000000000001E-3</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37">
         <v>31.6</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>51</v>
       </c>
       <c r="B38" s="1">
         <v>955085</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38">
         <v>3477</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38">
         <v>3.6410000000000001E-3</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38">
         <v>30.7</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>52</v>
       </c>
       <c r="B39" s="1">
         <v>951608</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39">
         <v>3765</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39">
         <v>3.9560000000000003E-3</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39">
         <v>29.9</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>53</v>
       </c>
       <c r="B40" s="1">
         <v>947843</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40">
         <v>4077</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40">
         <v>4.3010000000000001E-3</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>54</v>
       </c>
       <c r="B41" s="1">
         <v>943766</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41">
         <v>4418</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41">
         <v>4.6810000000000003E-3</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41">
         <v>28.1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>55</v>
       </c>
       <c r="B42" s="1">
         <v>939348</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42">
         <v>4744</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42">
         <v>5.0499999999999998E-3</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42">
         <v>27.2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>56</v>
       </c>
       <c r="B43" s="1">
         <v>934604</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43">
         <v>5106</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43">
         <v>5.463E-3</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43">
         <v>26.4</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>57</v>
       </c>
       <c r="B44" s="1">
         <v>929498</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44">
         <v>5507</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44">
         <v>5.9249999999999997E-3</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E44">
         <v>25.5</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>58</v>
       </c>
       <c r="B45" s="1">
         <v>923991</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45">
         <v>5952</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45">
         <v>6.4419999999999998E-3</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45">
         <v>24.6</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>59</v>
       </c>
       <c r="B46" s="1">
         <v>918039</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46">
         <v>6444</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46">
         <v>7.0190000000000001E-3</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46">
         <v>23.8</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>60</v>
       </c>
       <c r="B47" s="1">
         <v>911595</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47">
         <v>6988</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47">
         <v>7.6660000000000001E-3</v>
       </c>
-      <c r="E47" s="2">
+      <c r="E47">
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>61</v>
       </c>
       <c r="B48" s="1">
         <v>904607</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48">
         <v>7588</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48">
         <v>8.3879999999999996E-3</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E48">
         <v>22.1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>62</v>
       </c>
       <c r="B49" s="1">
         <v>897019</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49">
         <v>8250</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D49">
         <v>9.1970000000000003E-3</v>
       </c>
-      <c r="E49" s="2">
+      <c r="E49">
         <v>21.3</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>63</v>
       </c>
       <c r="B50" s="1">
         <v>888769</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50">
         <v>9134</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50">
         <v>1.0277E-2</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E50">
         <v>20.5</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>64</v>
       </c>
       <c r="B51" s="1">
         <v>879635</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51">
         <v>10078</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D51">
         <v>1.1457E-2</v>
       </c>
-      <c r="E51" s="2">
+      <c r="E51">
         <v>19.7</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>65</v>
       </c>
       <c r="B52" s="1">
         <v>869557</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52">
         <v>11080</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D52">
         <v>1.2742E-2</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E52">
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>66</v>
       </c>
       <c r="B53" s="1">
         <v>858477</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53">
         <v>12143</v>
       </c>
-      <c r="D53" s="2">
+      <c r="D53">
         <v>1.4145E-2</v>
       </c>
-      <c r="E53" s="2">
+      <c r="E53">
         <v>18.2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>67</v>
       </c>
       <c r="B54" s="1">
         <v>846334</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54">
         <v>13265</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D54">
         <v>1.5672999999999999E-2</v>
       </c>
-      <c r="E54" s="2">
+      <c r="E54">
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>68</v>
       </c>
       <c r="B55" s="1">
         <v>833069</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55">
         <v>14446</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D55">
         <v>1.7340999999999999E-2</v>
       </c>
-      <c r="E55" s="2">
+      <c r="E55">
         <v>16.7</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>69</v>
       </c>
       <c r="B56" s="1">
         <v>818623</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56">
         <v>15683</v>
       </c>
-      <c r="D56" s="2">
+      <c r="D56">
         <v>1.9158000000000001E-2</v>
       </c>
-      <c r="E56" s="2">
+      <c r="E56">
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>70</v>
       </c>
       <c r="B57" s="1">
         <v>802940</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57">
         <v>16972</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D57">
         <v>2.1137E-2</v>
       </c>
-      <c r="E57" s="2">
+      <c r="E57">
         <v>15.3</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>71</v>
       </c>
       <c r="B58" s="1">
         <v>785968</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58">
         <v>18310</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58">
         <v>2.3296000000000001E-2</v>
       </c>
-      <c r="E58" s="2">
+      <c r="E58">
         <v>14.6</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>72</v>
       </c>
       <c r="B59" s="1">
         <v>767658</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59">
         <v>19688</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D59">
         <v>2.5647E-2</v>
       </c>
-      <c r="E59" s="2">
+      <c r="E59">
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>73</v>
       </c>
       <c r="B60" s="1">
         <v>747970</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60">
         <v>21098</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D60">
         <v>2.8206999999999999E-2</v>
       </c>
-      <c r="E60" s="2">
+      <c r="E60">
         <v>13.3</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>74</v>
       </c>
       <c r="B61" s="1">
         <v>726872</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61">
         <v>22530</v>
       </c>
-      <c r="D61" s="2">
+      <c r="D61">
         <v>3.0995999999999999E-2</v>
       </c>
-      <c r="E61" s="2">
+      <c r="E61">
         <v>12.7</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>75</v>
       </c>
       <c r="B62" s="1">
         <v>704342</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62">
         <v>23970</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D62">
         <v>3.4032E-2</v>
       </c>
-      <c r="E62" s="2">
+      <c r="E62">
         <v>12.1</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>76</v>
       </c>
       <c r="B63" s="1">
         <v>680372</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63">
         <v>25.402000000000001</v>
       </c>
-      <c r="D63" s="2">
+      <c r="D63">
         <v>3.7335E-2</v>
       </c>
-      <c r="E63" s="2">
+      <c r="E63">
         <v>11.5</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>77</v>
       </c>
       <c r="B64" s="1">
         <v>654970</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64">
         <v>26808</v>
       </c>
-      <c r="D64" s="2">
+      <c r="D64">
         <v>4.0930000000000001E-2</v>
       </c>
-      <c r="E64" s="2">
+      <c r="E64">
         <v>10.9</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>78</v>
       </c>
       <c r="B65" s="1">
         <v>628162</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65">
         <v>28168</v>
       </c>
-      <c r="D65" s="2">
+      <c r="D65">
         <v>4.4842E-2</v>
       </c>
-      <c r="E65" s="2">
+      <c r="E65">
         <v>10.4</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>79</v>
       </c>
       <c r="B66" s="1">
         <v>599994</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66">
         <v>29456</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D66">
         <v>4.9093999999999999E-2</v>
       </c>
-      <c r="E66" s="2">
+      <c r="E66">
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>80</v>
       </c>
       <c r="B67" s="1">
         <v>570538</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67">
         <v>30646</v>
       </c>
-      <c r="D67" s="2">
+      <c r="D67">
         <v>5.3713999999999998E-2</v>
       </c>
-      <c r="E67" s="2">
+      <c r="E67">
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>81</v>
       </c>
       <c r="B68" s="1">
         <v>539892</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68">
         <v>31711</v>
       </c>
-      <c r="D68" s="2">
+      <c r="D68">
         <v>5.8735999999999997E-2</v>
       </c>
-      <c r="E68" s="2">
+      <c r="E68">
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>82</v>
       </c>
       <c r="B69" s="1">
         <v>508181</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69">
         <v>32619</v>
       </c>
-      <c r="D69" s="2">
+      <c r="D69">
         <v>6.4187999999999995E-2</v>
       </c>
-      <c r="E69" s="2">
+      <c r="E69">
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>83</v>
       </c>
       <c r="B70" s="1">
         <v>475562</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70">
         <v>33340</v>
       </c>
-      <c r="D70" s="2">
+      <c r="D70">
         <v>7.0107000000000003E-2</v>
       </c>
-      <c r="E70" s="2">
+      <c r="E70">
         <v>7.8</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>84</v>
       </c>
       <c r="B71" s="1">
         <v>442222</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71">
         <v>33841</v>
       </c>
-      <c r="D71" s="2">
+      <c r="D71">
         <v>7.6524999999999996E-2</v>
       </c>
-      <c r="E71" s="2">
+      <c r="E71">
         <v>7.4</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>85</v>
       </c>
       <c r="B72" s="1">
         <v>408381</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C72">
         <v>34093</v>
       </c>
-      <c r="D72" s="2">
+      <c r="D72">
         <v>8.3483000000000002E-2</v>
       </c>
-      <c r="E72" s="2">
+      <c r="E72">
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>86</v>
       </c>
       <c r="B73" s="1">
         <v>374288</v>
       </c>
-      <c r="C73" s="2">
+      <c r="C73">
         <v>34069</v>
       </c>
-      <c r="D73" s="2">
+      <c r="D73">
         <v>9.1023000000000007E-2</v>
       </c>
-      <c r="E73" s="2">
+      <c r="E73">
         <v>6.6</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>87</v>
       </c>
       <c r="B74" s="1">
         <v>340219</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C74">
         <v>33745</v>
       </c>
-      <c r="D74" s="2">
+      <c r="D74">
         <v>9.9185999999999996E-2</v>
       </c>
-      <c r="E74" s="2">
+      <c r="E74">
         <v>6.2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>88</v>
       </c>
       <c r="B75" s="1">
         <v>306474</v>
       </c>
-      <c r="C75" s="2">
+      <c r="C75">
         <v>33103</v>
       </c>
-      <c r="D75" s="2">
+      <c r="D75">
         <v>0.108012</v>
       </c>
-      <c r="E75" s="2">
+      <c r="E75">
         <v>5.8</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>89</v>
       </c>
       <c r="B76" s="1">
         <v>273371</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C76">
         <v>32136</v>
       </c>
-      <c r="D76" s="2">
+      <c r="D76">
         <v>0.11755500000000001</v>
       </c>
-      <c r="E76" s="2">
+      <c r="E76">
         <v>5.4</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>90</v>
       </c>
       <c r="B77" s="1">
         <v>241235</v>
       </c>
-      <c r="C77" s="2">
+      <c r="C77">
         <v>30844</v>
       </c>
-      <c r="D77" s="2">
+      <c r="D77">
         <v>0.127859</v>
       </c>
-      <c r="E77" s="2">
+      <c r="E77">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>91</v>
       </c>
       <c r="B78" s="1">
         <v>210391</v>
       </c>
-      <c r="C78" s="2">
+      <c r="C78">
         <v>29239</v>
       </c>
-      <c r="D78" s="2">
+      <c r="D78">
         <v>0.13897499999999999</v>
       </c>
-      <c r="E78" s="2">
+      <c r="E78">
         <v>4.8</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>92</v>
       </c>
       <c r="B79" s="1">
         <v>181152</v>
       </c>
-      <c r="C79" s="2">
+      <c r="C79">
         <v>27344</v>
       </c>
-      <c r="D79" s="2">
+      <c r="D79">
         <v>0.150945</v>
       </c>
-      <c r="E79" s="2">
+      <c r="E79">
         <v>4.5</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>93</v>
       </c>
       <c r="B80" s="1">
         <v>153808</v>
       </c>
-      <c r="C80" s="2">
+      <c r="C80">
         <v>25199</v>
       </c>
-      <c r="D80" s="2">
+      <c r="D80">
         <v>0.16383400000000001</v>
       </c>
-      <c r="E80" s="2">
+      <c r="E80">
         <v>4.2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>94</v>
       </c>
       <c r="B81" s="1">
         <v>128609</v>
       </c>
-      <c r="C81" s="2">
+      <c r="C81">
         <v>22851</v>
       </c>
-      <c r="D81" s="2">
+      <c r="D81">
         <v>0.177678</v>
       </c>
-      <c r="E81" s="2">
+      <c r="E81">
         <v>3.9</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>95</v>
       </c>
       <c r="B82" s="1">
         <v>105758</v>
       </c>
-      <c r="C82" s="2">
+      <c r="C82">
         <v>20363</v>
       </c>
-      <c r="D82" s="2">
+      <c r="D82">
         <v>0.19254299999999999</v>
       </c>
-      <c r="E82" s="2">
+      <c r="E82">
         <v>3.6</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>96</v>
       </c>
       <c r="B83" s="1">
         <v>85395</v>
       </c>
-      <c r="C83" s="2">
+      <c r="C83">
         <v>17839</v>
       </c>
-      <c r="D83" s="2">
+      <c r="D83">
         <v>0.2089</v>
       </c>
-      <c r="E83" s="2">
+      <c r="E83">
         <v>3.3</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>97</v>
       </c>
       <c r="B84" s="1">
         <v>67556</v>
       </c>
-      <c r="C84" s="2">
+      <c r="C84">
         <v>15350</v>
       </c>
-      <c r="D84" s="2">
+      <c r="D84">
         <v>0.227219</v>
       </c>
-      <c r="E84" s="2">
+      <c r="E84">
         <v>3.1</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>98</v>
       </c>
       <c r="B85" s="1">
         <v>52206</v>
       </c>
-      <c r="C85" s="2">
+      <c r="C85">
         <v>12921</v>
       </c>
-      <c r="D85" s="2">
+      <c r="D85">
         <v>0.2475</v>
       </c>
-      <c r="E85" s="2">
+      <c r="E85">
         <v>2.9</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>99</v>
       </c>
       <c r="B86" s="1">
         <v>39285</v>
       </c>
-      <c r="C86" s="2">
+      <c r="C86">
         <v>10597</v>
       </c>
-      <c r="D86" s="2">
+      <c r="D86">
         <v>0.26974700000000001</v>
       </c>
-      <c r="E86" s="2">
+      <c r="E86">
         <v>2.6</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>100</v>
       </c>
       <c r="B87" s="1">
         <v>28688</v>
       </c>
-      <c r="C87" s="2">
+      <c r="C87">
         <v>8433</v>
       </c>
-      <c r="D87" s="2">
+      <c r="D87">
         <v>0.293956</v>
       </c>
-      <c r="E87" s="2">
+      <c r="E87">
         <v>2.4</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>101</v>
       </c>
       <c r="B88" s="1">
         <v>20255</v>
       </c>
-      <c r="C88" s="2">
+      <c r="C88">
         <v>6484</v>
       </c>
-      <c r="D88" s="2">
+      <c r="D88">
         <v>0.32011800000000001</v>
       </c>
-      <c r="E88" s="2">
+      <c r="E88">
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>102</v>
       </c>
       <c r="B89" s="1">
         <v>13771</v>
       </c>
-      <c r="C89" s="2">
+      <c r="C89">
         <v>4796</v>
       </c>
-      <c r="D89" s="2">
+      <c r="D89">
         <v>0.34826800000000002</v>
       </c>
-      <c r="E89" s="2">
+      <c r="E89">
         <v>2.1</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>103</v>
       </c>
       <c r="B90" s="1">
         <v>8975</v>
       </c>
-      <c r="C90" s="2">
+      <c r="C90">
         <v>3395</v>
       </c>
-      <c r="D90" s="2">
+      <c r="D90">
         <v>0.37827300000000003</v>
       </c>
-      <c r="E90" s="2">
+      <c r="E90">
         <v>1.9</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>104</v>
       </c>
       <c r="B91" s="1">
         <v>5580</v>
       </c>
-      <c r="C91" s="2">
+      <c r="C91">
         <v>2290</v>
       </c>
-      <c r="D91" s="2">
+      <c r="D91">
         <v>0.41039399999999998</v>
       </c>
-      <c r="E91" s="2">
+      <c r="E91">
         <v>1.7</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>105</v>
       </c>
       <c r="B92" s="1">
         <v>3290</v>
       </c>
-      <c r="C92" s="2">
+      <c r="C92">
         <v>1.462</v>
       </c>
-      <c r="D92" s="2">
+      <c r="D92">
         <v>0.44437700000000002</v>
       </c>
-      <c r="E92" s="2">
+      <c r="E92">
         <v>1.6</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>106</v>
       </c>
       <c r="B93" s="1">
         <v>1828</v>
       </c>
-      <c r="C93" s="2">
+      <c r="C93">
         <v>878</v>
       </c>
-      <c r="D93" s="2">
+      <c r="D93">
         <v>0.48030600000000001</v>
       </c>
-      <c r="E93" s="2">
+      <c r="E93">
         <v>1.4</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>107</v>
       </c>
       <c r="B94" s="1">
         <v>950</v>
       </c>
-      <c r="C94" s="2">
+      <c r="C94">
         <v>492</v>
       </c>
-      <c r="D94" s="2">
+      <c r="D94">
         <v>0.51789499999999999</v>
       </c>
-      <c r="E94" s="2">
+      <c r="E94">
         <v>1.3</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>108</v>
       </c>
       <c r="B95" s="1">
         <v>458</v>
       </c>
-      <c r="C95" s="2">
+      <c r="C95">
         <v>256</v>
       </c>
-      <c r="D95" s="2">
+      <c r="D95">
         <v>0.558952</v>
       </c>
-      <c r="E95" s="2">
+      <c r="E95">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>109</v>
       </c>
       <c r="B96" s="1">
         <v>202</v>
       </c>
-      <c r="C96" s="2">
+      <c r="C96">
         <v>121</v>
       </c>
-      <c r="D96" s="2">
+      <c r="D96">
         <v>0.59901000000000004</v>
       </c>
-      <c r="E96" s="2">
+      <c r="E96">
         <v>0.9</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>110</v>
       </c>
       <c r="B97" s="1">
         <v>81</v>
       </c>
-      <c r="C97" s="2">
+      <c r="C97">
         <v>81</v>
       </c>
-      <c r="D97" s="2">
+      <c r="D97">
         <v>1</v>
       </c>
-      <c r="E97" s="2">
+      <c r="E97">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>